<commit_message>
Textgrid Type pts. 42-44
</commit_message>
<xml_diff>
--- a/REPSWITCH_List.xlsx
+++ b/REPSWITCH_List.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\experiment1\Experimental_scripts\Instructions_grids\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\experiment1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E1E4D8C-E9C9-42F1-959B-A7A267A8F3FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEE4475E-653B-40D2-AC5D-9EE8FEFE40E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="912" windowWidth="17736" windowHeight="12048" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pilots" sheetId="3" r:id="rId1"/>
@@ -588,6 +588,16 @@
   </cellStyles>
   <dxfs count="25">
     <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -607,16 +617,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1117,17 +1117,17 @@
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{6A81B45A-EDC9-4FF5-8258-8648C067C16F}" name="Participant"/>
     <tableColumn id="5" xr3:uid="{23D0A20D-D062-4D9A-A44D-D77B8E1CBB39}" name="Name"/>
-    <tableColumn id="10" xr3:uid="{706E71AC-2B72-418D-A17F-64B513C711DC}" name="ID" dataDxfId="4" totalsRowDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{7D21F159-CC51-40B5-A3A9-2FC35A1E3DC7}" name="Code" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{706E71AC-2B72-418D-A17F-64B513C711DC}" name="ID" dataDxfId="8" totalsRowDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{7D21F159-CC51-40B5-A3A9-2FC35A1E3DC7}" name="Code" dataDxfId="6" totalsRowDxfId="5"/>
     <tableColumn id="2" xr3:uid="{0F7B8E20-170E-4530-BD6F-052C78EE98C3}" name="Version "/>
     <tableColumn id="3" xr3:uid="{C9573F81-3819-423D-82CC-5ABB8EA301BD}" name="List"/>
-    <tableColumn id="6" xr3:uid="{27B86DF5-6EF1-41B1-A9EC-9F0F5F275ADB}" name="Language_test" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{27B86DF5-6EF1-41B1-A9EC-9F0F5F275ADB}" name="Language_test" dataDxfId="4" totalsRowDxfId="3"/>
     <tableColumn id="9" xr3:uid="{89FF1955-3050-4A09-8388-44DB3C7BAF8D}" name="Date"/>
     <tableColumn id="13" xr3:uid="{0353A7A6-5360-4B04-A7A6-65360A0DB44E}" name="Notes"/>
     <tableColumn id="14" xr3:uid="{4580F522-AB7C-463E-B145-EBE3420458C5}" name="FechaNacimiento"/>
-    <tableColumn id="15" xr3:uid="{E351B0AB-595F-4765-9989-9C66FD2C2557}" name="Sexo" dataDxfId="8" totalsRowDxfId="7"/>
+    <tableColumn id="15" xr3:uid="{E351B0AB-595F-4765-9989-9C66FD2C2557}" name="Sexo" dataDxfId="2" totalsRowDxfId="1"/>
     <tableColumn id="16" xr3:uid="{C57334FC-C4FE-4E54-8FCF-DE2F9464D89B}" name="Supertecleador"/>
-    <tableColumn id="8" xr3:uid="{4C118AC6-F397-4959-8D77-72283767A378}" name="Type_speed" totalsRowFunction="custom" totalsRowDxfId="6">
+    <tableColumn id="8" xr3:uid="{4C118AC6-F397-4959-8D77-72283767A378}" name="Type_speed" totalsRowFunction="custom" totalsRowDxfId="0">
       <totalsRowFormula>AVERAGE(Table1[Type_speed])</totalsRowFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{298D1824-20FA-4582-B3FC-14618C8BA8DE}" name="Type_accuracy" totalsRowFunction="custom">
@@ -1595,7 +1595,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{395959F8-4BC5-4C1E-B558-7BF10E8FA50A}">
   <dimension ref="A1:S54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Textgrid Type pts. 45-49
</commit_message>
<xml_diff>
--- a/REPSWITCH_List.xlsx
+++ b/REPSWITCH_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\experiment1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEE4475E-653B-40D2-AC5D-9EE8FEFE40E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B80891-37AB-4019-B314-191E5A7B47A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1116" yWindow="912" windowWidth="17736" windowHeight="12048" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pilots" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="129">
   <si>
     <t>Participant</t>
   </si>
@@ -387,9 +387,6 @@
     <t>Unai Roca</t>
   </si>
   <si>
-    <t>A bit sleepy. Can do the caja.</t>
-  </si>
-  <si>
     <t>Has a cut on her right index. No issue in typing. Took off the bandage. Can do the caja.</t>
   </si>
   <si>
@@ -421,6 +418,12 @@
   </si>
   <si>
     <t>check sex for NR</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>A bit sleepy. Can do the caja. Heavy breathing during typing trials. Many modality errors during typing trials.</t>
   </si>
 </sst>
 </file>
@@ -552,7 +555,6 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -562,11 +564,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -582,19 +580,37 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="34">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -606,7 +622,26 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -614,6 +649,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1089,48 +1125,49 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D7725C54-BC3C-4F16-BE30-EAEFD1E6A889}" name="Table2" displayName="Table2" ref="A1:N3" totalsRowShown="0" headerRowDxfId="24" dataDxfId="22" headerRowBorderDxfId="23" tableBorderDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D7725C54-BC3C-4F16-BE30-EAEFD1E6A889}" name="Table2" displayName="Table2" ref="A1:N3" totalsRowShown="0" headerRowDxfId="33" dataDxfId="31" headerRowBorderDxfId="32" tableBorderDxfId="30">
   <autoFilter ref="A1:N3" xr:uid="{D7725C54-BC3C-4F16-BE30-EAEFD1E6A889}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{7424B4AF-20BB-4956-A693-DA5C2E491F93}" name="Nº" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{D26CEDE0-6675-4478-AE1C-23ABA5C453CA}" name="NOMBRE" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{EFE7765A-783D-40C2-88ED-FBD03D4624CF}" name="ID" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{44B7B9A7-3620-4B2C-AA1F-A445ABB5A4AB}" name="CODE" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{53BF4CCF-E2C8-4075-828B-045D44DC2B5B}" name="DATE" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{7424B4AF-20BB-4956-A693-DA5C2E491F93}" name="Nº" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{D26CEDE0-6675-4478-AE1C-23ABA5C453CA}" name="NOMBRE" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{EFE7765A-783D-40C2-88ED-FBD03D4624CF}" name="ID" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{44B7B9A7-3620-4B2C-AA1F-A445ABB5A4AB}" name="CODE" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{53BF4CCF-E2C8-4075-828B-045D44DC2B5B}" name="DATE" dataDxfId="25"/>
     <tableColumn id="13" xr3:uid="{1015A516-CB69-4FC3-87A7-C4A13E267A67}" name="FechaNacimiento"/>
     <tableColumn id="14" xr3:uid="{EA8F05D9-3EE2-477E-9DA0-F765608E29F0}" name="Sexo"/>
-    <tableColumn id="6" xr3:uid="{1B290470-E23F-485F-AC08-FFFEAC9F056D}" name="VERSION" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{F0145F60-BB11-4B87-9FCD-BDAB0F3EDDB5}" name="LIST" dataDxfId="14"/>
-    <tableColumn id="8" xr3:uid="{2F9D02AD-A101-4502-9045-CD9C9E13C48F}" name="CAB" dataDxfId="13"/>
-    <tableColumn id="9" xr3:uid="{85FF814B-2A7B-432F-8DAE-5AB34249AEB5}" name="RA" dataDxfId="12"/>
-    <tableColumn id="10" xr3:uid="{0FC227E0-1B27-4152-863B-2CB8F32204E6}" name="INCIDENCES" dataDxfId="11"/>
-    <tableColumn id="12" xr3:uid="{503F2B95-E846-4929-AB22-0B04260E6C24}" name="Type_speed" dataDxfId="10"/>
-    <tableColumn id="11" xr3:uid="{EDCB596B-12D3-4EB1-8CF7-AAF9A3093A4F}" name="Type_accuracy" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{1B290470-E23F-485F-AC08-FFFEAC9F056D}" name="VERSION" dataDxfId="24"/>
+    <tableColumn id="7" xr3:uid="{F0145F60-BB11-4B87-9FCD-BDAB0F3EDDB5}" name="LIST" dataDxfId="23"/>
+    <tableColumn id="8" xr3:uid="{2F9D02AD-A101-4502-9045-CD9C9E13C48F}" name="CAB" dataDxfId="22"/>
+    <tableColumn id="9" xr3:uid="{85FF814B-2A7B-432F-8DAE-5AB34249AEB5}" name="RA" dataDxfId="21"/>
+    <tableColumn id="10" xr3:uid="{0FC227E0-1B27-4152-863B-2CB8F32204E6}" name="INCIDENCES" dataDxfId="20"/>
+    <tableColumn id="12" xr3:uid="{503F2B95-E846-4929-AB22-0B04260E6C24}" name="Type_speed" dataDxfId="19"/>
+    <tableColumn id="11" xr3:uid="{EDCB596B-12D3-4EB1-8CF7-AAF9A3093A4F}" name="Type_accuracy" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{894C102C-C055-48F5-AE8E-D7DEA7C38926}" name="Table1" displayName="Table1" ref="A1:N51" totalsRowCount="1">
-  <autoFilter ref="A1:N50" xr:uid="{894C102C-C055-48F5-AE8E-D7DEA7C38926}"/>
-  <tableColumns count="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{894C102C-C055-48F5-AE8E-D7DEA7C38926}" name="Table1" displayName="Table1" ref="A1:O51" totalsRowCount="1">
+  <autoFilter ref="A1:O50" xr:uid="{894C102C-C055-48F5-AE8E-D7DEA7C38926}"/>
+  <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{6A81B45A-EDC9-4FF5-8258-8648C067C16F}" name="Participant"/>
     <tableColumn id="5" xr3:uid="{23D0A20D-D062-4D9A-A44D-D77B8E1CBB39}" name="Name"/>
-    <tableColumn id="10" xr3:uid="{706E71AC-2B72-418D-A17F-64B513C711DC}" name="ID" dataDxfId="8" totalsRowDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{7D21F159-CC51-40B5-A3A9-2FC35A1E3DC7}" name="Code" dataDxfId="6" totalsRowDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{706E71AC-2B72-418D-A17F-64B513C711DC}" name="ID" dataDxfId="17" totalsRowDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{7D21F159-CC51-40B5-A3A9-2FC35A1E3DC7}" name="Code" dataDxfId="16" totalsRowDxfId="7"/>
     <tableColumn id="2" xr3:uid="{0F7B8E20-170E-4530-BD6F-052C78EE98C3}" name="Version "/>
     <tableColumn id="3" xr3:uid="{C9573F81-3819-423D-82CC-5ABB8EA301BD}" name="List"/>
-    <tableColumn id="6" xr3:uid="{27B86DF5-6EF1-41B1-A9EC-9F0F5F275ADB}" name="Language_test" dataDxfId="4" totalsRowDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{27B86DF5-6EF1-41B1-A9EC-9F0F5F275ADB}" name="Language_test" dataDxfId="15" totalsRowDxfId="6"/>
     <tableColumn id="9" xr3:uid="{89FF1955-3050-4A09-8388-44DB3C7BAF8D}" name="Date"/>
     <tableColumn id="13" xr3:uid="{0353A7A6-5360-4B04-A7A6-65360A0DB44E}" name="Notes"/>
-    <tableColumn id="14" xr3:uid="{4580F522-AB7C-463E-B145-EBE3420458C5}" name="FechaNacimiento"/>
-    <tableColumn id="15" xr3:uid="{E351B0AB-595F-4765-9989-9C66FD2C2557}" name="Sexo" dataDxfId="2" totalsRowDxfId="1"/>
-    <tableColumn id="16" xr3:uid="{C57334FC-C4FE-4E54-8FCF-DE2F9464D89B}" name="Supertecleador"/>
-    <tableColumn id="8" xr3:uid="{4C118AC6-F397-4959-8D77-72283767A378}" name="Type_speed" totalsRowFunction="custom" totalsRowDxfId="0">
+    <tableColumn id="14" xr3:uid="{4580F522-AB7C-463E-B145-EBE3420458C5}" name="FechaNacimiento" dataDxfId="14" totalsRowDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{692F1DCA-E4E0-468B-99F8-ADCD8D7F70E7}" name="Age" dataDxfId="13" totalsRowDxfId="4"/>
+    <tableColumn id="15" xr3:uid="{E351B0AB-595F-4765-9989-9C66FD2C2557}" name="Sexo" dataDxfId="12" totalsRowDxfId="3"/>
+    <tableColumn id="16" xr3:uid="{C57334FC-C4FE-4E54-8FCF-DE2F9464D89B}" name="Supertecleador" dataDxfId="11" totalsRowDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{4C118AC6-F397-4959-8D77-72283767A378}" name="Type_speed" totalsRowFunction="custom" dataDxfId="10" totalsRowDxfId="1">
       <totalsRowFormula>AVERAGE(Table1[Type_speed])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{298D1824-20FA-4582-B3FC-14618C8BA8DE}" name="Type_accuracy" totalsRowFunction="custom">
+    <tableColumn id="7" xr3:uid="{298D1824-20FA-4582-B3FC-14618C8BA8DE}" name="Type_accuracy" totalsRowFunction="custom" dataDxfId="9" totalsRowDxfId="0">
       <totalsRowFormula>AVERAGE(Table1[Type_accuracy])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -1513,7 +1550,7 @@
       <c r="F2" s="7">
         <v>36624</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="14" t="s">
         <v>83</v>
       </c>
       <c r="H2" s="5">
@@ -1557,7 +1594,7 @@
       <c r="F3" s="11">
         <v>37810</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="15" t="s">
         <v>85</v>
       </c>
       <c r="H3" s="8">
@@ -1593,43 +1630,43 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{395959F8-4BC5-4C1E-B558-7BF10E8FA50A}">
-  <dimension ref="A1:S54"/>
+  <dimension ref="A1:T54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="25.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" style="17" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="17"/>
+    <col min="3" max="3" width="12" style="16" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="16"/>
     <col min="6" max="6" width="9.6640625" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="17"/>
+    <col min="7" max="7" width="8.88671875" style="16"/>
     <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="31.88671875" customWidth="1"/>
-    <col min="10" max="10" width="13.44140625" customWidth="1"/>
-    <col min="11" max="11" width="13.44140625" style="17" customWidth="1"/>
-    <col min="12" max="12" width="10.77734375" customWidth="1"/>
-    <col min="13" max="13" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="13.44140625" style="16" customWidth="1"/>
+    <col min="13" max="13" width="10.77734375" style="16" customWidth="1"/>
+    <col min="14" max="14" width="10.77734375" style="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.88671875" style="16"/>
+    <col min="16" max="16" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
@@ -1638,7 +1675,7 @@
       <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="16" t="s">
         <v>13</v>
       </c>
       <c r="H1" t="s">
@@ -1647,33 +1684,36 @@
       <c r="I1" t="s">
         <v>44</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="K1" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="L1" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="L1" t="s">
-        <v>118</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="M1" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="N1" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" s="16" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="21">
+      <c r="C2" s="18">
         <v>9383</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="19" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="1">
@@ -1682,40 +1722,41 @@
       <c r="F2" s="1">
         <v>1</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="19" t="s">
         <v>21</v>
       </c>
       <c r="H2" s="3">
         <v>45240</v>
       </c>
       <c r="I2" s="11"/>
-      <c r="J2" s="11">
+      <c r="J2" s="23">
         <v>36910</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="23"/>
+      <c r="L2" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="L2" t="s">
-        <v>119</v>
-      </c>
-      <c r="M2">
+      <c r="M2" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="N2" s="16">
         <v>38.72</v>
       </c>
-      <c r="N2">
+      <c r="O2" s="16">
         <v>98.84</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="21">
+      <c r="C3" s="18">
         <v>11777</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="19" t="s">
         <v>53</v>
       </c>
       <c r="E3" s="1">
@@ -1724,42 +1765,43 @@
       <c r="F3" s="1">
         <v>1</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="19" t="s">
         <v>21</v>
       </c>
       <c r="H3" s="3">
         <v>45240</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="J3" s="11">
+        <v>124</v>
+      </c>
+      <c r="J3" s="23">
         <v>36978</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="K3" s="23"/>
+      <c r="L3" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="L3" t="s">
-        <v>119</v>
-      </c>
-      <c r="M3">
+      <c r="M3" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="N3" s="16">
         <v>30.76</v>
       </c>
-      <c r="N3">
+      <c r="O3" s="16">
         <v>98.76</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="18">
         <v>8424</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="19" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="1">
@@ -1768,42 +1810,43 @@
       <c r="F4" s="1">
         <v>2</v>
       </c>
-      <c r="G4" s="22" t="s">
+      <c r="G4" s="19" t="s">
         <v>21</v>
       </c>
       <c r="H4" s="3">
         <v>45240</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="J4" s="11">
+        <v>124</v>
+      </c>
+      <c r="J4" s="23">
         <v>36484</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="K4" s="23"/>
+      <c r="L4" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="L4" t="s">
-        <v>119</v>
-      </c>
-      <c r="M4">
+      <c r="M4" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="N4" s="16">
         <v>33.520000000000003</v>
       </c>
-      <c r="N4">
+      <c r="O4" s="16">
         <v>95.04</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="18">
         <v>11787</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="19" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="1">
@@ -1812,40 +1855,41 @@
       <c r="F5" s="1">
         <v>2</v>
       </c>
-      <c r="G5" s="22" t="s">
+      <c r="G5" s="19" t="s">
         <v>22</v>
       </c>
       <c r="H5" s="3">
         <v>45246</v>
       </c>
       <c r="I5" s="11"/>
-      <c r="J5" s="11">
+      <c r="J5" s="23">
         <v>36631</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="K5" s="23"/>
+      <c r="L5" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="L5" t="s">
-        <v>120</v>
-      </c>
-      <c r="M5">
+      <c r="M5" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="N5" s="16">
         <v>43.32</v>
       </c>
-      <c r="N5">
+      <c r="O5" s="16">
         <v>95.94</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="18">
         <v>8542</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="19" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="1">
@@ -1854,7 +1898,7 @@
       <c r="F6" s="1">
         <v>3</v>
       </c>
-      <c r="G6" s="22" t="s">
+      <c r="G6" s="19" t="s">
         <v>43</v>
       </c>
       <c r="H6" s="3">
@@ -1863,33 +1907,34 @@
       <c r="I6" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="11">
+      <c r="J6" s="23">
         <v>33073</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="K6" s="23"/>
+      <c r="L6" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="L6" t="s">
-        <v>120</v>
-      </c>
-      <c r="M6">
+      <c r="M6" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="N6" s="16">
         <v>35.6</v>
       </c>
-      <c r="N6">
+      <c r="O6" s="16">
         <v>93.18</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C7" s="18">
         <v>11587</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="19" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="1">
@@ -1898,7 +1943,7 @@
       <c r="F7" s="1">
         <v>3</v>
       </c>
-      <c r="G7" s="22" t="s">
+      <c r="G7" s="19" t="s">
         <v>46</v>
       </c>
       <c r="H7" s="3">
@@ -1907,33 +1952,34 @@
       <c r="I7" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="J7" s="11">
+      <c r="J7" s="23">
         <v>38338</v>
       </c>
-      <c r="K7" s="8" t="s">
+      <c r="K7" s="23"/>
+      <c r="L7" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="L7" t="s">
-        <v>119</v>
-      </c>
-      <c r="M7">
+      <c r="M7" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="N7" s="16">
         <v>34.479999999999997</v>
       </c>
-      <c r="N7">
+      <c r="O7" s="16">
         <v>89.92</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="23">
+      <c r="C8" s="20">
         <v>11082</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="19" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="1">
@@ -1942,7 +1988,7 @@
       <c r="F8" s="1">
         <v>4</v>
       </c>
-      <c r="G8" s="22" t="s">
+      <c r="G8" s="19" t="s">
         <v>48</v>
       </c>
       <c r="H8" s="12">
@@ -1951,33 +1997,34 @@
       <c r="I8" t="s">
         <v>50</v>
       </c>
-      <c r="J8" s="14">
+      <c r="J8" s="24">
         <v>37166</v>
       </c>
-      <c r="K8" s="8" t="s">
+      <c r="K8" s="24"/>
+      <c r="L8" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="L8" t="s">
-        <v>119</v>
-      </c>
-      <c r="M8">
+      <c r="M8" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="N8" s="16">
         <v>34.479999999999997</v>
       </c>
-      <c r="N8">
+      <c r="O8" s="16">
         <v>89.92</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="23">
+      <c r="C9" s="20">
         <v>11000</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="19" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="1">
@@ -1986,7 +2033,7 @@
       <c r="F9" s="1">
         <v>4</v>
       </c>
-      <c r="G9" s="22" t="s">
+      <c r="G9" s="19" t="s">
         <v>22</v>
       </c>
       <c r="H9" s="12">
@@ -1995,33 +2042,34 @@
       <c r="I9" t="s">
         <v>21</v>
       </c>
-      <c r="J9" s="14">
+      <c r="J9" s="24">
         <v>37264</v>
       </c>
-      <c r="K9" s="8" t="s">
+      <c r="K9" s="24"/>
+      <c r="L9" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="L9" t="s">
-        <v>119</v>
-      </c>
-      <c r="M9">
+      <c r="M9" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="N9" s="16">
         <v>32.799999999999997</v>
       </c>
-      <c r="N9">
+      <c r="O9" s="16">
         <v>93.48</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="23">
+      <c r="C10" s="20">
         <v>11893</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="19" t="s">
         <v>11</v>
       </c>
       <c r="E10" s="1">
@@ -2030,7 +2078,7 @@
       <c r="F10" s="1">
         <v>1</v>
       </c>
-      <c r="G10" s="22" t="s">
+      <c r="G10" s="19" t="s">
         <v>43</v>
       </c>
       <c r="H10" s="12">
@@ -2039,33 +2087,34 @@
       <c r="I10" t="s">
         <v>59</v>
       </c>
-      <c r="J10" s="14">
+      <c r="J10" s="24">
         <v>37200</v>
       </c>
-      <c r="K10" s="17" t="s">
+      <c r="K10" s="24"/>
+      <c r="L10" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="L10" t="s">
-        <v>120</v>
-      </c>
-      <c r="M10">
+      <c r="M10" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="N10" s="16">
         <v>38.6</v>
       </c>
-      <c r="N10">
+      <c r="O10" s="16">
         <v>91.66</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="23">
+      <c r="C11" s="20">
         <v>10439</v>
       </c>
-      <c r="D11" s="22">
+      <c r="D11" s="19">
         <v>100201</v>
       </c>
       <c r="E11" s="1">
@@ -2074,7 +2123,7 @@
       <c r="F11" s="1">
         <v>1</v>
       </c>
-      <c r="G11" s="22" t="s">
+      <c r="G11" s="19" t="s">
         <v>46</v>
       </c>
       <c r="H11" s="12">
@@ -2083,33 +2132,34 @@
       <c r="I11" t="s">
         <v>65</v>
       </c>
-      <c r="J11" s="14">
+      <c r="J11" s="24">
         <v>36893</v>
       </c>
-      <c r="K11" s="17" t="s">
+      <c r="K11" s="24"/>
+      <c r="L11" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="L11" t="s">
-        <v>119</v>
-      </c>
-      <c r="M11">
+      <c r="M11" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="N11" s="16">
         <v>32.6</v>
       </c>
-      <c r="N11">
+      <c r="O11" s="16">
         <v>91.14</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="23">
+      <c r="C12" s="20">
         <v>11570</v>
       </c>
-      <c r="D12" s="22">
+      <c r="D12" s="19">
         <v>110102</v>
       </c>
       <c r="E12" s="1">
@@ -2118,39 +2168,40 @@
       <c r="F12" s="1">
         <v>2</v>
       </c>
-      <c r="G12" s="22" t="s">
+      <c r="G12" s="19" t="s">
         <v>48</v>
       </c>
       <c r="H12" s="12">
         <v>45257</v>
       </c>
-      <c r="J12" s="14">
+      <c r="J12" s="24">
         <v>37880</v>
       </c>
-      <c r="K12" s="17" t="s">
+      <c r="K12" s="24"/>
+      <c r="L12" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="L12" t="s">
-        <v>119</v>
-      </c>
-      <c r="M12">
+      <c r="M12" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="N12" s="16">
         <v>40.799999999999997</v>
       </c>
-      <c r="N12">
+      <c r="O12" s="16">
         <v>98.18</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="23">
+      <c r="C13" s="20">
         <v>9754</v>
       </c>
-      <c r="D13" s="22">
+      <c r="D13" s="19">
         <v>120202</v>
       </c>
       <c r="E13" s="1">
@@ -2159,7 +2210,7 @@
       <c r="F13" s="1">
         <v>2</v>
       </c>
-      <c r="G13" s="22" t="s">
+      <c r="G13" s="19" t="s">
         <v>22</v>
       </c>
       <c r="H13" s="12">
@@ -2168,33 +2219,34 @@
       <c r="I13" t="s">
         <v>51</v>
       </c>
-      <c r="J13" s="14">
+      <c r="J13" s="24">
         <v>37460</v>
       </c>
-      <c r="K13" s="17" t="s">
+      <c r="K13" s="24"/>
+      <c r="L13" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="L13" t="s">
-        <v>119</v>
-      </c>
-      <c r="M13">
+      <c r="M13" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="N13" s="16">
         <v>45.88</v>
       </c>
-      <c r="N13">
+      <c r="O13" s="16">
         <v>95.66</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C14" s="23">
+      <c r="C14" s="20">
         <v>10344</v>
       </c>
-      <c r="D14" s="22">
+      <c r="D14" s="19">
         <v>130103</v>
       </c>
       <c r="E14" s="1">
@@ -2203,39 +2255,40 @@
       <c r="F14" s="1">
         <v>3</v>
       </c>
-      <c r="G14" s="22" t="s">
+      <c r="G14" s="19" t="s">
         <v>43</v>
       </c>
       <c r="H14" s="12">
         <v>45257</v>
       </c>
-      <c r="J14" s="14">
+      <c r="J14" s="24">
         <v>37504</v>
       </c>
-      <c r="K14" s="17" t="s">
+      <c r="K14" s="24"/>
+      <c r="L14" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="L14" t="s">
-        <v>119</v>
-      </c>
-      <c r="M14">
+      <c r="M14" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="N14" s="16">
         <v>40.32</v>
       </c>
-      <c r="N14">
+      <c r="O14" s="16">
         <v>93.64</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C15" s="23">
+      <c r="C15" s="20">
         <v>11614</v>
       </c>
-      <c r="D15" s="22">
+      <c r="D15" s="19">
         <v>140203</v>
       </c>
       <c r="E15" s="1">
@@ -2244,42 +2297,43 @@
       <c r="F15" s="1">
         <v>3</v>
       </c>
-      <c r="G15" s="22" t="s">
+      <c r="G15" s="19" t="s">
         <v>46</v>
       </c>
       <c r="H15" s="12">
         <v>45258</v>
       </c>
-      <c r="J15" s="14">
+      <c r="J15" s="24">
         <v>38214</v>
       </c>
-      <c r="K15" s="17" t="s">
+      <c r="K15" s="24"/>
+      <c r="L15" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="L15" t="s">
-        <v>119</v>
-      </c>
-      <c r="M15">
+      <c r="M15" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="N15" s="16">
         <v>34.04</v>
       </c>
-      <c r="N15">
+      <c r="O15" s="16">
         <v>95.1</v>
       </c>
-      <c r="S15" t="s">
+      <c r="T15" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C16" s="23">
+      <c r="C16" s="20">
         <v>11782</v>
       </c>
-      <c r="D16" s="22">
+      <c r="D16" s="19">
         <v>150104</v>
       </c>
       <c r="E16" s="1">
@@ -2288,39 +2342,40 @@
       <c r="F16" s="1">
         <v>4</v>
       </c>
-      <c r="G16" s="22" t="s">
+      <c r="G16" s="19" t="s">
         <v>48</v>
       </c>
       <c r="H16" s="12">
         <v>45258</v>
       </c>
-      <c r="J16" s="14">
+      <c r="J16" s="24">
         <v>37691</v>
       </c>
-      <c r="K16" s="17" t="s">
+      <c r="K16" s="24"/>
+      <c r="L16" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="L16" t="s">
-        <v>119</v>
-      </c>
-      <c r="M16">
+      <c r="M16" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="N16" s="16">
         <v>39.520000000000003</v>
       </c>
-      <c r="N16">
+      <c r="O16" s="16">
         <v>94.88</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="23">
+      <c r="C17" s="20">
         <v>11481</v>
       </c>
-      <c r="D17" s="22">
+      <c r="D17" s="19">
         <v>160204</v>
       </c>
       <c r="E17" s="1">
@@ -2329,7 +2384,7 @@
       <c r="F17" s="1">
         <v>4</v>
       </c>
-      <c r="G17" s="22" t="s">
+      <c r="G17" s="19" t="s">
         <v>22</v>
       </c>
       <c r="H17" s="12">
@@ -2338,33 +2393,34 @@
       <c r="I17" t="s">
         <v>64</v>
       </c>
-      <c r="J17" s="14">
+      <c r="J17" s="24">
         <v>34028</v>
       </c>
-      <c r="K17" s="17" t="s">
+      <c r="K17" s="24"/>
+      <c r="L17" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="L17" t="s">
-        <v>120</v>
-      </c>
-      <c r="M17">
+      <c r="M17" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="N17" s="16">
         <v>40.68</v>
       </c>
-      <c r="N17">
+      <c r="O17" s="16">
         <v>93.42</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C18" s="23">
+      <c r="C18" s="20">
         <v>11438</v>
       </c>
-      <c r="D18" s="22">
+      <c r="D18" s="19">
         <v>170101</v>
       </c>
       <c r="E18" s="1">
@@ -2373,7 +2429,7 @@
       <c r="F18" s="1">
         <v>1</v>
       </c>
-      <c r="G18" s="22" t="s">
+      <c r="G18" s="19" t="s">
         <v>43</v>
       </c>
       <c r="H18" s="12">
@@ -2382,33 +2438,34 @@
       <c r="I18" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="J18" s="11">
+      <c r="J18" s="23">
         <v>38244</v>
       </c>
-      <c r="K18" s="17" t="s">
+      <c r="K18" s="23"/>
+      <c r="L18" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="L18" t="s">
-        <v>119</v>
-      </c>
-      <c r="M18">
+      <c r="M18" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="N18" s="16">
         <v>44.4</v>
       </c>
-      <c r="N18">
+      <c r="O18" s="16">
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="C19" s="24">
+      <c r="C19" s="21">
         <v>2293</v>
       </c>
-      <c r="D19" s="22">
+      <c r="D19" s="19">
         <v>180201</v>
       </c>
       <c r="E19" s="1">
@@ -2417,7 +2474,7 @@
       <c r="F19" s="1">
         <v>1</v>
       </c>
-      <c r="G19" s="22" t="s">
+      <c r="G19" s="19" t="s">
         <v>46</v>
       </c>
       <c r="H19" s="12">
@@ -2426,33 +2483,34 @@
       <c r="I19" t="s">
         <v>101</v>
       </c>
-      <c r="J19" s="14">
+      <c r="J19" s="24">
         <v>32903</v>
       </c>
-      <c r="K19" s="17" t="s">
+      <c r="K19" s="24"/>
+      <c r="L19" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="L19" t="s">
-        <v>119</v>
-      </c>
-      <c r="M19">
+      <c r="M19" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="N19" s="16">
         <v>35.08</v>
       </c>
-      <c r="N19">
+      <c r="O19" s="16">
         <v>96.42</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C20" s="21">
+      <c r="C20" s="18">
         <v>9818</v>
       </c>
-      <c r="D20" s="22">
+      <c r="D20" s="19">
         <v>190102</v>
       </c>
       <c r="E20" s="1">
@@ -2461,7 +2519,7 @@
       <c r="F20" s="1">
         <v>2</v>
       </c>
-      <c r="G20" s="22" t="s">
+      <c r="G20" s="19" t="s">
         <v>48</v>
       </c>
       <c r="H20" s="12">
@@ -2470,33 +2528,34 @@
       <c r="I20" t="s">
         <v>71</v>
       </c>
-      <c r="J20" s="14">
+      <c r="J20" s="24">
         <v>37433</v>
       </c>
-      <c r="K20" s="17" t="s">
+      <c r="K20" s="24"/>
+      <c r="L20" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="L20" t="s">
-        <v>119</v>
-      </c>
-      <c r="M20">
+      <c r="M20" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="N20" s="16">
         <v>32.72</v>
       </c>
-      <c r="N20">
+      <c r="O20" s="16">
         <v>81.86</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C21" s="21">
+      <c r="C21" s="18">
         <v>10983</v>
       </c>
-      <c r="D21" s="22">
+      <c r="D21" s="19">
         <v>200202</v>
       </c>
       <c r="E21" s="1">
@@ -2505,39 +2564,40 @@
       <c r="F21" s="1">
         <v>2</v>
       </c>
-      <c r="G21" s="22" t="s">
+      <c r="G21" s="19" t="s">
         <v>22</v>
       </c>
       <c r="H21" s="12">
         <v>45260</v>
       </c>
-      <c r="J21" s="14">
+      <c r="J21" s="24">
         <v>37936</v>
       </c>
-      <c r="K21" s="17" t="s">
+      <c r="K21" s="24"/>
+      <c r="L21" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="L21" t="s">
-        <v>119</v>
-      </c>
-      <c r="M21">
+      <c r="M21" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="N21" s="16">
         <v>38.159999999999997</v>
       </c>
-      <c r="N21">
+      <c r="O21" s="16">
         <v>97.36</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C22" s="21">
+      <c r="C22" s="18">
         <v>11478</v>
       </c>
-      <c r="D22" s="22">
+      <c r="D22" s="19">
         <v>210103</v>
       </c>
       <c r="E22" s="1">
@@ -2546,7 +2606,7 @@
       <c r="F22" s="1">
         <v>3</v>
       </c>
-      <c r="G22" s="22" t="s">
+      <c r="G22" s="19" t="s">
         <v>43</v>
       </c>
       <c r="H22" s="12">
@@ -2555,33 +2615,34 @@
       <c r="I22" t="s">
         <v>76</v>
       </c>
-      <c r="J22" s="14">
+      <c r="J22" s="24">
         <v>34393</v>
       </c>
-      <c r="K22" s="17" t="s">
+      <c r="K22" s="24"/>
+      <c r="L22" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="L22" t="s">
-        <v>120</v>
-      </c>
-      <c r="M22">
+      <c r="M22" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="N22" s="16">
         <v>55.64</v>
       </c>
-      <c r="N22">
+      <c r="O22" s="16">
         <v>97.48</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C23" s="23">
+      <c r="C23" s="20">
         <v>10464</v>
       </c>
-      <c r="D23" s="22">
+      <c r="D23" s="19">
         <v>220203</v>
       </c>
       <c r="E23" s="1">
@@ -2590,39 +2651,40 @@
       <c r="F23" s="1">
         <v>3</v>
       </c>
-      <c r="G23" s="22" t="s">
+      <c r="G23" s="19" t="s">
         <v>46</v>
       </c>
       <c r="H23" s="12">
         <v>45261</v>
       </c>
-      <c r="J23" s="14">
+      <c r="J23" s="24">
         <v>35659</v>
       </c>
-      <c r="K23" s="17" t="s">
+      <c r="K23" s="24"/>
+      <c r="L23" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="L23" t="s">
-        <v>120</v>
-      </c>
-      <c r="M23">
+      <c r="M23" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="N23" s="16">
         <v>52.28</v>
       </c>
-      <c r="N23">
+      <c r="O23" s="16">
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C24" s="23">
+      <c r="C24" s="20">
         <v>10637</v>
       </c>
-      <c r="D24" s="22">
+      <c r="D24" s="19">
         <v>230104</v>
       </c>
       <c r="E24" s="1">
@@ -2631,7 +2693,7 @@
       <c r="F24" s="1">
         <v>4</v>
       </c>
-      <c r="G24" s="22" t="s">
+      <c r="G24" s="19" t="s">
         <v>48</v>
       </c>
       <c r="H24" s="12">
@@ -2640,33 +2702,34 @@
       <c r="I24" t="s">
         <v>51</v>
       </c>
-      <c r="J24" s="14">
+      <c r="J24" s="24">
         <v>37869</v>
       </c>
-      <c r="K24" s="17" t="s">
+      <c r="K24" s="24"/>
+      <c r="L24" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="L24" t="s">
-        <v>119</v>
-      </c>
-      <c r="M24">
+      <c r="M24" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="N24" s="16">
         <v>34.72</v>
       </c>
-      <c r="N24">
+      <c r="O24" s="16">
         <v>90.66</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C25" s="23">
+      <c r="C25" s="20">
         <v>10443</v>
       </c>
-      <c r="D25" s="22">
+      <c r="D25" s="19">
         <v>240204</v>
       </c>
       <c r="E25" s="1">
@@ -2675,7 +2738,7 @@
       <c r="F25" s="1">
         <v>4</v>
       </c>
-      <c r="G25" s="22" t="s">
+      <c r="G25" s="19" t="s">
         <v>22</v>
       </c>
       <c r="H25" s="12">
@@ -2684,36 +2747,37 @@
       <c r="I25" t="s">
         <v>102</v>
       </c>
-      <c r="J25" s="14">
+      <c r="J25" s="24">
         <v>37670</v>
       </c>
-      <c r="K25" s="17" t="s">
+      <c r="K25" s="24"/>
+      <c r="L25" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="L25" t="s">
-        <v>120</v>
-      </c>
-      <c r="M25">
+      <c r="M25" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="N25" s="16">
         <v>50.16</v>
       </c>
-      <c r="N25">
+      <c r="O25" s="16">
         <v>97.14</v>
       </c>
-      <c r="S25" t="s">
+      <c r="T25" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="C26" s="24">
+      <c r="C26" s="21">
         <v>11512</v>
       </c>
-      <c r="D26" s="22">
+      <c r="D26" s="19">
         <v>250101</v>
       </c>
       <c r="E26" s="1">
@@ -2722,39 +2786,40 @@
       <c r="F26" s="1">
         <v>1</v>
       </c>
-      <c r="G26" s="22" t="s">
+      <c r="G26" s="19" t="s">
         <v>43</v>
       </c>
       <c r="H26" s="12">
         <v>45264</v>
       </c>
-      <c r="J26" s="14">
+      <c r="J26" s="24">
         <v>37838</v>
       </c>
-      <c r="K26" s="17" t="s">
+      <c r="K26" s="24"/>
+      <c r="L26" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="L26" t="s">
-        <v>119</v>
-      </c>
-      <c r="M26">
+      <c r="M26" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="N26" s="16">
         <v>34.4</v>
       </c>
-      <c r="N26">
+      <c r="O26" s="16">
         <v>95.88</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C27" s="21">
+      <c r="C27" s="18">
         <v>11124</v>
       </c>
-      <c r="D27" s="22">
+      <c r="D27" s="19">
         <v>260201</v>
       </c>
       <c r="E27" s="1">
@@ -2763,39 +2828,40 @@
       <c r="F27" s="1">
         <v>1</v>
       </c>
-      <c r="G27" s="22" t="s">
+      <c r="G27" s="19" t="s">
         <v>46</v>
       </c>
       <c r="H27" s="12">
         <v>45264</v>
       </c>
-      <c r="J27" s="14">
+      <c r="J27" s="24">
         <v>37040</v>
       </c>
-      <c r="K27" s="17" t="s">
+      <c r="K27" s="24"/>
+      <c r="L27" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="L27" t="s">
-        <v>119</v>
-      </c>
-      <c r="M27">
+      <c r="M27" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="N27" s="16">
         <v>40.72</v>
       </c>
-      <c r="N27">
+      <c r="O27" s="16">
         <v>93.08</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C28" s="21">
+      <c r="C28" s="18">
         <v>11600</v>
       </c>
-      <c r="D28" s="22">
+      <c r="D28" s="19">
         <v>270102</v>
       </c>
       <c r="E28" s="1">
@@ -2804,42 +2870,43 @@
       <c r="F28" s="1">
         <v>2</v>
       </c>
-      <c r="G28" s="22" t="s">
+      <c r="G28" s="19" t="s">
         <v>48</v>
       </c>
       <c r="H28" s="12">
         <v>45264</v>
       </c>
       <c r="I28" t="s">
-        <v>123</v>
-      </c>
-      <c r="J28" s="14">
+        <v>122</v>
+      </c>
+      <c r="J28" s="24">
         <v>38142</v>
       </c>
-      <c r="K28" s="17" t="s">
+      <c r="K28" s="24"/>
+      <c r="L28" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="L28" t="s">
-        <v>119</v>
-      </c>
-      <c r="M28">
+      <c r="M28" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="N28" s="16">
         <v>41.68</v>
       </c>
-      <c r="N28">
+      <c r="O28" s="16">
         <v>89.06</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C29" s="21">
+      <c r="C29" s="18">
         <v>3061</v>
       </c>
-      <c r="D29" s="22">
+      <c r="D29" s="19">
         <v>280202</v>
       </c>
       <c r="E29" s="1">
@@ -2848,42 +2915,43 @@
       <c r="F29" s="1">
         <v>2</v>
       </c>
-      <c r="G29" s="22" t="s">
+      <c r="G29" s="19" t="s">
         <v>22</v>
       </c>
       <c r="H29" s="12">
         <v>45264</v>
       </c>
       <c r="I29" t="s">
-        <v>122</v>
-      </c>
-      <c r="J29" s="14">
+        <v>121</v>
+      </c>
+      <c r="J29" s="24">
         <v>33365</v>
       </c>
-      <c r="K29" s="17" t="s">
+      <c r="K29" s="24"/>
+      <c r="L29" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="L29" t="s">
-        <v>119</v>
-      </c>
-      <c r="M29">
+      <c r="M29" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="N29" s="16">
         <v>33.6</v>
       </c>
-      <c r="N29">
+      <c r="O29" s="16">
         <v>87.76</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C30" s="21">
+      <c r="C30" s="18">
         <v>11527</v>
       </c>
-      <c r="D30" s="22">
+      <c r="D30" s="19">
         <v>290103</v>
       </c>
       <c r="E30" s="1">
@@ -2892,7 +2960,7 @@
       <c r="F30" s="1">
         <v>3</v>
       </c>
-      <c r="G30" s="22" t="s">
+      <c r="G30" s="19" t="s">
         <v>43</v>
       </c>
       <c r="H30" s="12">
@@ -2901,33 +2969,34 @@
       <c r="I30" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="J30" s="14">
+      <c r="J30" s="24">
         <v>37810</v>
       </c>
-      <c r="K30" s="17" t="s">
+      <c r="K30" s="24"/>
+      <c r="L30" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="L30" t="s">
-        <v>119</v>
-      </c>
-      <c r="M30">
+      <c r="M30" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="N30" s="16">
         <v>43.68</v>
       </c>
-      <c r="N30">
+      <c r="O30" s="16">
         <v>88.68</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C31" s="21">
+      <c r="C31" s="18">
         <v>2317</v>
       </c>
-      <c r="D31" s="22">
+      <c r="D31" s="19">
         <v>300203</v>
       </c>
       <c r="E31" s="1">
@@ -2936,42 +3005,43 @@
       <c r="F31" s="1">
         <v>3</v>
       </c>
-      <c r="G31" s="22" t="s">
+      <c r="G31" s="19" t="s">
         <v>46</v>
       </c>
       <c r="H31" s="12">
         <v>45265</v>
       </c>
       <c r="I31" t="s">
-        <v>121</v>
-      </c>
-      <c r="J31" s="14">
+        <v>120</v>
+      </c>
+      <c r="J31" s="24">
         <v>33146</v>
       </c>
-      <c r="K31" s="17" t="s">
+      <c r="K31" s="24"/>
+      <c r="L31" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="L31" t="s">
-        <v>120</v>
-      </c>
-      <c r="M31">
+      <c r="M31" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="N31" s="16">
         <v>50</v>
       </c>
-      <c r="N31">
+      <c r="O31" s="16">
         <v>95.12</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C32" s="21">
+      <c r="C32" s="18">
         <v>8175</v>
       </c>
-      <c r="D32" s="22">
+      <c r="D32" s="19">
         <v>310104</v>
       </c>
       <c r="E32" s="1">
@@ -2980,39 +3050,40 @@
       <c r="F32" s="1">
         <v>4</v>
       </c>
-      <c r="G32" s="22" t="s">
+      <c r="G32" s="19" t="s">
         <v>48</v>
       </c>
       <c r="H32" s="12">
         <v>45265</v>
       </c>
-      <c r="J32" s="14">
+      <c r="J32" s="24">
         <v>32922</v>
       </c>
-      <c r="K32" s="17" t="s">
+      <c r="K32" s="24"/>
+      <c r="L32" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="L32" t="s">
-        <v>119</v>
-      </c>
-      <c r="M32">
+      <c r="M32" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="N32" s="16">
         <v>43.4</v>
       </c>
-      <c r="N32">
+      <c r="O32" s="16">
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C33" s="21">
+      <c r="C33" s="18">
         <v>1697</v>
       </c>
-      <c r="D33" s="22">
+      <c r="D33" s="19">
         <v>320204</v>
       </c>
       <c r="E33" s="1">
@@ -3021,39 +3092,40 @@
       <c r="F33" s="1">
         <v>4</v>
       </c>
-      <c r="G33" s="22" t="s">
+      <c r="G33" s="19" t="s">
         <v>22</v>
       </c>
       <c r="H33" s="12">
         <v>45265</v>
       </c>
-      <c r="J33" s="14">
+      <c r="J33" s="24">
         <v>32661</v>
       </c>
-      <c r="K33" s="17" t="s">
+      <c r="K33" s="24"/>
+      <c r="L33" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="L33" t="s">
-        <v>119</v>
-      </c>
-      <c r="M33">
+      <c r="M33" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="N33" s="16">
         <v>55.92</v>
       </c>
-      <c r="N33">
+      <c r="O33" s="16">
         <v>92.66</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C34" s="23">
+      <c r="C34" s="20">
         <v>9039</v>
       </c>
-      <c r="D34" s="22">
+      <c r="D34" s="19">
         <v>330101</v>
       </c>
       <c r="E34" s="1">
@@ -3062,39 +3134,40 @@
       <c r="F34" s="1">
         <v>1</v>
       </c>
-      <c r="G34" s="22" t="s">
+      <c r="G34" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="H34" s="19">
+      <c r="H34" s="17">
         <v>45271</v>
       </c>
-      <c r="J34" s="14">
+      <c r="J34" s="24">
         <v>35705</v>
       </c>
-      <c r="K34" s="17" t="s">
+      <c r="K34" s="24"/>
+      <c r="L34" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="L34" t="s">
-        <v>120</v>
-      </c>
-      <c r="M34">
+      <c r="M34" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="N34" s="16">
         <v>43.32</v>
       </c>
-      <c r="N34">
+      <c r="O34" s="16">
         <v>95.3</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C35" s="21">
+      <c r="C35" s="18">
         <v>10010</v>
       </c>
-      <c r="D35" s="22">
+      <c r="D35" s="19">
         <v>340201</v>
       </c>
       <c r="E35" s="1">
@@ -3103,42 +3176,43 @@
       <c r="F35" s="1">
         <v>1</v>
       </c>
-      <c r="G35" s="22" t="s">
+      <c r="G35" s="19" t="s">
         <v>46</v>
       </c>
       <c r="H35" s="3">
         <v>45272</v>
       </c>
       <c r="I35" t="s">
-        <v>124</v>
-      </c>
-      <c r="J35" s="14">
+        <v>123</v>
+      </c>
+      <c r="J35" s="24">
         <v>37475</v>
       </c>
-      <c r="K35" s="17" t="s">
+      <c r="K35" s="24"/>
+      <c r="L35" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="L35" t="s">
-        <v>119</v>
-      </c>
-      <c r="M35">
+      <c r="M35" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="N35" s="16">
         <v>43.88</v>
       </c>
-      <c r="N35">
+      <c r="O35" s="16">
         <v>95.3</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C36" s="21">
+      <c r="C36" s="18">
         <v>10415</v>
       </c>
-      <c r="D36" s="22">
+      <c r="D36" s="19">
         <v>350102</v>
       </c>
       <c r="E36" s="1">
@@ -3147,39 +3221,40 @@
       <c r="F36" s="1">
         <v>2</v>
       </c>
-      <c r="G36" s="22" t="s">
+      <c r="G36" s="19" t="s">
         <v>48</v>
       </c>
       <c r="H36" s="3">
         <v>45272</v>
       </c>
-      <c r="J36" s="14">
+      <c r="J36" s="24">
         <v>37515</v>
       </c>
-      <c r="K36" s="17" t="s">
+      <c r="K36" s="24"/>
+      <c r="L36" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="L36" t="s">
-        <v>119</v>
-      </c>
-      <c r="M36">
+      <c r="M36" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="N36" s="16">
         <v>45.76</v>
       </c>
-      <c r="N36">
+      <c r="O36" s="16">
         <v>92.12</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C37" s="21">
+      <c r="C37" s="18">
         <v>6729</v>
       </c>
-      <c r="D37" s="22">
+      <c r="D37" s="19">
         <v>360202</v>
       </c>
       <c r="E37" s="1">
@@ -3188,39 +3263,40 @@
       <c r="F37" s="1">
         <v>2</v>
       </c>
-      <c r="G37" s="22" t="s">
+      <c r="G37" s="19" t="s">
         <v>22</v>
       </c>
       <c r="H37" s="3">
         <v>45272</v>
       </c>
-      <c r="J37" s="14">
+      <c r="J37" s="24">
         <v>34059</v>
       </c>
-      <c r="K37" s="17" t="s">
+      <c r="K37" s="24"/>
+      <c r="L37" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="L37" t="s">
-        <v>119</v>
-      </c>
-      <c r="M37">
+      <c r="M37" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="N37" s="16">
         <v>36.200000000000003</v>
       </c>
-      <c r="N37">
+      <c r="O37" s="16">
         <v>98.38</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C38" s="21">
+      <c r="C38" s="18">
         <v>11066</v>
       </c>
-      <c r="D38" s="22">
+      <c r="D38" s="19">
         <v>370103</v>
       </c>
       <c r="E38" s="1">
@@ -3229,7 +3305,7 @@
       <c r="F38" s="1">
         <v>3</v>
       </c>
-      <c r="G38" s="22" t="s">
+      <c r="G38" s="19" t="s">
         <v>43</v>
       </c>
       <c r="H38" s="12">
@@ -3238,33 +3314,34 @@
       <c r="I38" t="s">
         <v>112</v>
       </c>
-      <c r="J38" s="14">
+      <c r="J38" s="24">
         <v>37152</v>
       </c>
-      <c r="K38" s="17" t="s">
+      <c r="K38" s="24"/>
+      <c r="L38" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="L38" t="s">
-        <v>119</v>
-      </c>
-      <c r="M38">
+      <c r="M38" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="N38" s="16">
         <v>40.159999999999997</v>
       </c>
-      <c r="N38">
+      <c r="O38" s="16">
         <v>90.36</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C39" s="23">
+      <c r="C39" s="20">
         <v>9245</v>
       </c>
-      <c r="D39" s="22">
+      <c r="D39" s="19">
         <v>380203</v>
       </c>
       <c r="E39" s="1">
@@ -3273,7 +3350,7 @@
       <c r="F39" s="1">
         <v>3</v>
       </c>
-      <c r="G39" s="22" t="s">
+      <c r="G39" s="19" t="s">
         <v>46</v>
       </c>
       <c r="H39" s="12">
@@ -3282,33 +3359,34 @@
       <c r="I39" t="s">
         <v>99</v>
       </c>
-      <c r="J39" s="14">
+      <c r="J39" s="24">
         <v>36607</v>
       </c>
-      <c r="K39" s="17" t="s">
+      <c r="K39" s="24"/>
+      <c r="L39" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="L39" t="s">
-        <v>119</v>
-      </c>
-      <c r="M39">
+      <c r="M39" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="N39" s="16">
         <v>38.68</v>
       </c>
-      <c r="N39">
+      <c r="O39" s="16">
         <v>95.02</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C40" s="23">
+      <c r="C40" s="20">
         <v>11067</v>
       </c>
-      <c r="D40" s="22">
+      <c r="D40" s="19">
         <v>390104</v>
       </c>
       <c r="E40" s="1">
@@ -3317,39 +3395,40 @@
       <c r="F40" s="1">
         <v>4</v>
       </c>
-      <c r="G40" s="22" t="s">
+      <c r="G40" s="19" t="s">
         <v>48</v>
       </c>
       <c r="H40" s="12">
         <v>45273</v>
       </c>
-      <c r="J40" s="14">
+      <c r="J40" s="24">
         <v>35101</v>
       </c>
-      <c r="K40" s="17" t="s">
+      <c r="K40" s="24"/>
+      <c r="L40" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="L40" t="s">
-        <v>120</v>
-      </c>
-      <c r="M40">
+      <c r="M40" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="N40" s="16">
         <v>66.52</v>
       </c>
-      <c r="N40">
+      <c r="O40" s="16">
         <v>98</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C41" s="23">
+      <c r="C41" s="20">
         <v>8819</v>
       </c>
-      <c r="D41" s="22">
+      <c r="D41" s="19">
         <v>400204</v>
       </c>
       <c r="E41" s="1">
@@ -3358,39 +3437,40 @@
       <c r="F41" s="1">
         <v>4</v>
       </c>
-      <c r="G41" s="22" t="s">
+      <c r="G41" s="19" t="s">
         <v>22</v>
       </c>
       <c r="H41" s="12">
         <v>45273</v>
       </c>
-      <c r="J41" s="14">
+      <c r="J41" s="24">
         <v>35856</v>
       </c>
-      <c r="K41" s="17" t="s">
+      <c r="K41" s="24"/>
+      <c r="L41" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="L41" t="s">
-        <v>120</v>
-      </c>
-      <c r="M41">
+      <c r="M41" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="N41" s="16">
         <v>52.04</v>
       </c>
-      <c r="N41">
+      <c r="O41" s="16">
         <v>98.58</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>41</v>
       </c>
       <c r="B42" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="C42" s="24">
+      <c r="C42" s="21">
         <v>6210</v>
       </c>
-      <c r="D42" s="22">
+      <c r="D42" s="19">
         <v>410101</v>
       </c>
       <c r="E42" s="1">
@@ -3399,39 +3479,40 @@
       <c r="F42" s="1">
         <v>1</v>
       </c>
-      <c r="G42" s="22" t="s">
+      <c r="G42" s="19" t="s">
         <v>43</v>
       </c>
       <c r="H42" s="12">
         <v>45274</v>
       </c>
-      <c r="J42" s="14">
+      <c r="J42" s="24">
         <v>35934</v>
       </c>
-      <c r="K42" s="17" t="s">
+      <c r="K42" s="24"/>
+      <c r="L42" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="L42" t="s">
-        <v>119</v>
-      </c>
-      <c r="M42">
+      <c r="M42" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="N42" s="16">
         <v>53.68</v>
       </c>
-      <c r="N42">
+      <c r="O42" s="16">
         <v>90.04</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C43" s="21">
+      <c r="C43" s="18">
         <v>10275</v>
       </c>
-      <c r="D43" s="22">
+      <c r="D43" s="19">
         <v>420201</v>
       </c>
       <c r="E43" s="1">
@@ -3440,7 +3521,7 @@
       <c r="F43" s="1">
         <v>1</v>
       </c>
-      <c r="G43" s="22" t="s">
+      <c r="G43" s="19" t="s">
         <v>46</v>
       </c>
       <c r="H43" s="12">
@@ -3449,33 +3530,34 @@
       <c r="I43" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="J43" s="14">
+      <c r="J43" s="24">
         <v>33061</v>
       </c>
-      <c r="K43" s="17" t="s">
+      <c r="K43" s="24"/>
+      <c r="L43" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="L43" t="s">
-        <v>119</v>
-      </c>
-      <c r="M43">
+      <c r="M43" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="N43" s="16">
         <v>40.200000000000003</v>
       </c>
-      <c r="N43">
+      <c r="O43" s="16">
         <v>94.42</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C44" s="23">
+      <c r="C44" s="20">
         <v>6835</v>
       </c>
-      <c r="D44" s="22">
+      <c r="D44" s="19">
         <v>430102</v>
       </c>
       <c r="E44" s="1">
@@ -3484,7 +3566,7 @@
       <c r="F44" s="1">
         <v>2</v>
       </c>
-      <c r="G44" s="22" t="s">
+      <c r="G44" s="19" t="s">
         <v>48</v>
       </c>
       <c r="H44" s="12">
@@ -3493,33 +3575,34 @@
       <c r="I44" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="J44" s="14">
+      <c r="J44" s="24">
         <v>33718</v>
       </c>
-      <c r="K44" s="17" t="s">
+      <c r="K44" s="24"/>
+      <c r="L44" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="L44" t="s">
-        <v>120</v>
-      </c>
-      <c r="M44">
+      <c r="M44" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="N44" s="16">
         <v>41.4</v>
       </c>
-      <c r="N44">
+      <c r="O44" s="16">
         <v>90.52</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>44</v>
       </c>
       <c r="B45" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="C45" s="24">
+      <c r="C45" s="21">
         <v>10964</v>
       </c>
-      <c r="D45" s="22">
+      <c r="D45" s="19">
         <v>440202</v>
       </c>
       <c r="E45" s="1">
@@ -3528,39 +3611,40 @@
       <c r="F45" s="1">
         <v>2</v>
       </c>
-      <c r="G45" s="22" t="s">
+      <c r="G45" s="19" t="s">
         <v>22</v>
       </c>
       <c r="H45" s="12">
         <v>45310</v>
       </c>
-      <c r="J45" s="14">
+      <c r="J45" s="24">
         <v>37441</v>
       </c>
-      <c r="K45" s="17" t="s">
+      <c r="K45" s="24"/>
+      <c r="L45" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="L45" t="s">
-        <v>119</v>
-      </c>
-      <c r="M45">
+      <c r="M45" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="N45" s="16">
         <v>41.8</v>
       </c>
-      <c r="N45">
+      <c r="O45" s="16">
         <v>98.06</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C46" s="23">
+      <c r="C46" s="20">
         <v>7789</v>
       </c>
-      <c r="D46" s="22">
+      <c r="D46" s="19">
         <v>450103</v>
       </c>
       <c r="E46" s="1">
@@ -3569,7 +3653,7 @@
       <c r="F46" s="1">
         <v>3</v>
       </c>
-      <c r="G46" s="22" t="s">
+      <c r="G46" s="19" t="s">
         <v>43</v>
       </c>
       <c r="H46" s="12">
@@ -3578,33 +3662,34 @@
       <c r="I46" t="s">
         <v>109</v>
       </c>
-      <c r="J46" s="14">
+      <c r="J46" s="24">
         <v>35886</v>
       </c>
-      <c r="K46" s="17" t="s">
+      <c r="K46" s="24"/>
+      <c r="L46" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="L46" t="s">
-        <v>120</v>
-      </c>
-      <c r="M46">
+      <c r="M46" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="N46" s="16">
         <v>51.2</v>
       </c>
-      <c r="N46">
+      <c r="O46" s="16">
         <v>97.62</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C47" s="23">
+      <c r="C47" s="20">
         <v>10942</v>
       </c>
-      <c r="D47" s="22">
+      <c r="D47" s="19">
         <v>460203</v>
       </c>
       <c r="E47" s="1">
@@ -3613,39 +3698,40 @@
       <c r="F47" s="1">
         <v>3</v>
       </c>
-      <c r="G47" s="22" t="s">
+      <c r="G47" s="19" t="s">
         <v>46</v>
       </c>
       <c r="H47" s="12">
         <v>45315</v>
       </c>
-      <c r="J47" s="14">
+      <c r="J47" s="24">
         <v>38070</v>
       </c>
-      <c r="K47" s="17" t="s">
+      <c r="K47" s="24"/>
+      <c r="L47" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="L47" t="s">
-        <v>119</v>
-      </c>
-      <c r="M47">
+      <c r="M47" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="N47" s="16">
         <v>35.72</v>
       </c>
-      <c r="N47">
+      <c r="O47" s="16">
         <v>95.58</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C48" s="21">
+      <c r="C48" s="18">
         <v>6020</v>
       </c>
-      <c r="D48" s="22">
+      <c r="D48" s="19">
         <v>470104</v>
       </c>
       <c r="E48" s="1">
@@ -3654,42 +3740,43 @@
       <c r="F48" s="1">
         <v>4</v>
       </c>
-      <c r="G48" s="22" t="s">
+      <c r="G48" s="19" t="s">
         <v>48</v>
       </c>
       <c r="H48" s="12">
         <v>45317</v>
       </c>
       <c r="I48" t="s">
-        <v>116</v>
-      </c>
-      <c r="J48" s="14">
+        <v>128</v>
+      </c>
+      <c r="J48" s="24">
         <v>36284</v>
       </c>
-      <c r="K48" s="17" t="s">
+      <c r="K48" s="24"/>
+      <c r="L48" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="L48" t="s">
-        <v>119</v>
-      </c>
-      <c r="M48">
+      <c r="M48" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="N48" s="16">
         <v>44.48</v>
       </c>
-      <c r="N48">
+      <c r="O48" s="16">
         <v>95.44</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C49" s="21">
+      <c r="C49" s="18">
         <v>10038</v>
       </c>
-      <c r="D49" s="22">
+      <c r="D49" s="19">
         <v>480204</v>
       </c>
       <c r="E49" s="1">
@@ -3698,42 +3785,43 @@
       <c r="F49" s="1">
         <v>4</v>
       </c>
-      <c r="G49" s="22" t="s">
+      <c r="G49" s="19" t="s">
         <v>22</v>
       </c>
       <c r="H49" s="12">
         <v>45317</v>
       </c>
       <c r="I49" t="s">
-        <v>117</v>
-      </c>
-      <c r="J49" s="14">
+        <v>116</v>
+      </c>
+      <c r="J49" s="24">
         <v>33386</v>
       </c>
-      <c r="K49" s="17" t="s">
+      <c r="K49" s="24"/>
+      <c r="L49" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="L49" t="s">
-        <v>120</v>
-      </c>
-      <c r="M49">
+      <c r="M49" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="N49" s="16">
         <v>61.56</v>
       </c>
-      <c r="N49">
+      <c r="O49" s="16">
         <v>95.84</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C50" s="21">
+      <c r="C50" s="18">
         <v>6477</v>
       </c>
-      <c r="D50" s="22" t="s">
+      <c r="D50" s="19" t="s">
         <v>111</v>
       </c>
       <c r="E50" s="1">
@@ -3742,48 +3830,49 @@
       <c r="F50" s="1">
         <v>1</v>
       </c>
-      <c r="G50" s="22" t="s">
+      <c r="G50" s="19" t="s">
         <v>43</v>
       </c>
       <c r="H50" s="12">
         <v>45317</v>
       </c>
-      <c r="J50" s="14">
+      <c r="J50" s="24">
         <v>34470</v>
       </c>
-      <c r="K50" s="17" t="s">
+      <c r="K50" s="24"/>
+      <c r="L50" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="L50" t="s">
-        <v>120</v>
-      </c>
-      <c r="M50">
+      <c r="M50" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="N50" s="16">
         <v>45.46</v>
       </c>
-      <c r="N50">
+      <c r="O50" s="16">
         <v>97.52</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D51" s="25"/>
-      <c r="G51" s="25"/>
-      <c r="M51" s="20">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D51" s="22"/>
+      <c r="G51" s="22"/>
+      <c r="N51" s="25">
         <f>AVERAGE(Table1[Type_speed])</f>
         <v>42.137551020408168</v>
       </c>
-      <c r="N51">
+      <c r="O51" s="16">
         <f>AVERAGE(Table1[Type_accuracy])</f>
         <v>93.98</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="J53" t="s">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J53" s="16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J54" s="16" t="s">
         <v>126</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="J54" t="s">
-        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Textgrid Speak pts. 42-44, Praat output files
</commit_message>
<xml_diff>
--- a/REPSWITCH_List.xlsx
+++ b/REPSWITCH_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\experiment1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B80891-37AB-4019-B314-191E5A7B47A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07782805-7D45-45CF-AE72-5928482AA2A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1116" yWindow="912" windowWidth="17736" windowHeight="12048" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pilots" sheetId="3" r:id="rId1"/>
@@ -351,9 +351,6 @@
     <t>Angelika Botero Montaña</t>
   </si>
   <si>
-    <t>Used words from South American Spanish in the familliarisation.</t>
-  </si>
-  <si>
     <t>Alejandro Muñoz Pérez</t>
   </si>
   <si>
@@ -424,6 +421,9 @@
   </si>
   <si>
     <t>A bit sleepy. Can do the caja. Heavy breathing during typing trials. Many modality errors during typing trials.</t>
+  </si>
+  <si>
+    <t>Used words from South American Spanish in the familliarisation. Slow Speak RTs.</t>
   </si>
 </sst>
 </file>
@@ -1632,8 +1632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{395959F8-4BC5-4C1E-B558-7BF10E8FA50A}">
   <dimension ref="A1:T54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1688,13 +1688,13 @@
         <v>81</v>
       </c>
       <c r="K1" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L1" s="16" t="s">
         <v>82</v>
       </c>
       <c r="M1" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="N1" s="16" t="s">
         <v>24</v>
@@ -1737,7 +1737,7 @@
         <v>85</v>
       </c>
       <c r="M2" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N2" s="16">
         <v>38.72</v>
@@ -1772,7 +1772,7 @@
         <v>45240</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J3" s="23">
         <v>36978</v>
@@ -1782,7 +1782,7 @@
         <v>85</v>
       </c>
       <c r="M3" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N3" s="16">
         <v>30.76</v>
@@ -1817,7 +1817,7 @@
         <v>45240</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J4" s="23">
         <v>36484</v>
@@ -1827,7 +1827,7 @@
         <v>85</v>
       </c>
       <c r="M4" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N4" s="16">
         <v>33.520000000000003</v>
@@ -1870,7 +1870,7 @@
         <v>85</v>
       </c>
       <c r="M5" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="N5" s="16">
         <v>43.32</v>
@@ -1915,7 +1915,7 @@
         <v>85</v>
       </c>
       <c r="M6" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="N6" s="16">
         <v>35.6</v>
@@ -1960,7 +1960,7 @@
         <v>85</v>
       </c>
       <c r="M7" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N7" s="16">
         <v>34.479999999999997</v>
@@ -2005,7 +2005,7 @@
         <v>85</v>
       </c>
       <c r="M8" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N8" s="16">
         <v>34.479999999999997</v>
@@ -2050,7 +2050,7 @@
         <v>85</v>
       </c>
       <c r="M9" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N9" s="16">
         <v>32.799999999999997</v>
@@ -2095,7 +2095,7 @@
         <v>83</v>
       </c>
       <c r="M10" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="N10" s="16">
         <v>38.6</v>
@@ -2140,7 +2140,7 @@
         <v>85</v>
       </c>
       <c r="M11" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N11" s="16">
         <v>32.6</v>
@@ -2182,7 +2182,7 @@
         <v>85</v>
       </c>
       <c r="M12" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N12" s="16">
         <v>40.799999999999997</v>
@@ -2227,7 +2227,7 @@
         <v>85</v>
       </c>
       <c r="M13" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N13" s="16">
         <v>45.88</v>
@@ -2269,7 +2269,7 @@
         <v>85</v>
       </c>
       <c r="M14" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N14" s="16">
         <v>40.32</v>
@@ -2311,7 +2311,7 @@
         <v>84</v>
       </c>
       <c r="M15" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N15" s="16">
         <v>34.04</v>
@@ -2356,7 +2356,7 @@
         <v>85</v>
       </c>
       <c r="M16" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N16" s="16">
         <v>39.520000000000003</v>
@@ -2401,7 +2401,7 @@
         <v>85</v>
       </c>
       <c r="M17" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="N17" s="16">
         <v>40.68</v>
@@ -2446,7 +2446,7 @@
         <v>85</v>
       </c>
       <c r="M18" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N18" s="16">
         <v>44.4</v>
@@ -2491,7 +2491,7 @@
         <v>85</v>
       </c>
       <c r="M19" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N19" s="16">
         <v>35.08</v>
@@ -2536,7 +2536,7 @@
         <v>85</v>
       </c>
       <c r="M20" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N20" s="16">
         <v>32.72</v>
@@ -2578,7 +2578,7 @@
         <v>85</v>
       </c>
       <c r="M21" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N21" s="16">
         <v>38.159999999999997</v>
@@ -2623,7 +2623,7 @@
         <v>83</v>
       </c>
       <c r="M22" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="N22" s="16">
         <v>55.64</v>
@@ -2665,7 +2665,7 @@
         <v>85</v>
       </c>
       <c r="M23" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="N23" s="16">
         <v>52.28</v>
@@ -2710,7 +2710,7 @@
         <v>85</v>
       </c>
       <c r="M24" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N24" s="16">
         <v>34.72</v>
@@ -2755,7 +2755,7 @@
         <v>85</v>
       </c>
       <c r="M25" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="N25" s="16">
         <v>50.16</v>
@@ -2800,7 +2800,7 @@
         <v>85</v>
       </c>
       <c r="M26" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N26" s="16">
         <v>34.4</v>
@@ -2842,7 +2842,7 @@
         <v>84</v>
       </c>
       <c r="M27" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N27" s="16">
         <v>40.72</v>
@@ -2877,7 +2877,7 @@
         <v>45264</v>
       </c>
       <c r="I28" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J28" s="24">
         <v>38142</v>
@@ -2887,7 +2887,7 @@
         <v>85</v>
       </c>
       <c r="M28" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N28" s="16">
         <v>41.68</v>
@@ -2922,7 +2922,7 @@
         <v>45264</v>
       </c>
       <c r="I29" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J29" s="24">
         <v>33365</v>
@@ -2932,7 +2932,7 @@
         <v>85</v>
       </c>
       <c r="M29" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N29" s="16">
         <v>33.6</v>
@@ -2977,7 +2977,7 @@
         <v>85</v>
       </c>
       <c r="M30" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N30" s="16">
         <v>43.68</v>
@@ -3012,7 +3012,7 @@
         <v>45265</v>
       </c>
       <c r="I31" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J31" s="24">
         <v>33146</v>
@@ -3022,7 +3022,7 @@
         <v>85</v>
       </c>
       <c r="M31" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="N31" s="16">
         <v>50</v>
@@ -3064,7 +3064,7 @@
         <v>85</v>
       </c>
       <c r="M32" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N32" s="16">
         <v>43.4</v>
@@ -3106,7 +3106,7 @@
         <v>85</v>
       </c>
       <c r="M33" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N33" s="16">
         <v>55.92</v>
@@ -3148,7 +3148,7 @@
         <v>84</v>
       </c>
       <c r="M34" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="N34" s="16">
         <v>43.32</v>
@@ -3183,7 +3183,7 @@
         <v>45272</v>
       </c>
       <c r="I35" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J35" s="24">
         <v>37475</v>
@@ -3193,7 +3193,7 @@
         <v>85</v>
       </c>
       <c r="M35" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N35" s="16">
         <v>43.88</v>
@@ -3235,7 +3235,7 @@
         <v>85</v>
       </c>
       <c r="M36" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N36" s="16">
         <v>45.76</v>
@@ -3277,7 +3277,7 @@
         <v>84</v>
       </c>
       <c r="M37" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N37" s="16">
         <v>36.200000000000003</v>
@@ -3312,7 +3312,7 @@
         <v>45273</v>
       </c>
       <c r="I38" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J38" s="24">
         <v>37152</v>
@@ -3322,7 +3322,7 @@
         <v>85</v>
       </c>
       <c r="M38" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N38" s="16">
         <v>40.159999999999997</v>
@@ -3367,7 +3367,7 @@
         <v>85</v>
       </c>
       <c r="M39" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N39" s="16">
         <v>38.68</v>
@@ -3409,7 +3409,7 @@
         <v>85</v>
       </c>
       <c r="M40" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="N40" s="16">
         <v>66.52</v>
@@ -3451,7 +3451,7 @@
         <v>85</v>
       </c>
       <c r="M41" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="N41" s="16">
         <v>52.04</v>
@@ -3493,7 +3493,7 @@
         <v>84</v>
       </c>
       <c r="M42" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N42" s="16">
         <v>53.68</v>
@@ -3528,7 +3528,7 @@
         <v>45307</v>
       </c>
       <c r="I43" s="9" t="s">
-        <v>104</v>
+        <v>128</v>
       </c>
       <c r="J43" s="24">
         <v>33061</v>
@@ -3538,7 +3538,7 @@
         <v>84</v>
       </c>
       <c r="M43" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N43" s="16">
         <v>40.200000000000003</v>
@@ -3552,7 +3552,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C44" s="20">
         <v>6835</v>
@@ -3573,7 +3573,7 @@
         <v>45309</v>
       </c>
       <c r="I44" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J44" s="24">
         <v>33718</v>
@@ -3583,7 +3583,7 @@
         <v>83</v>
       </c>
       <c r="M44" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="N44" s="16">
         <v>41.4</v>
@@ -3597,7 +3597,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C45" s="21">
         <v>10964</v>
@@ -3625,7 +3625,7 @@
         <v>84</v>
       </c>
       <c r="M45" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N45" s="16">
         <v>41.8</v>
@@ -3639,7 +3639,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C46" s="20">
         <v>7789</v>
@@ -3660,7 +3660,7 @@
         <v>45314</v>
       </c>
       <c r="I46" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J46" s="24">
         <v>35886</v>
@@ -3670,7 +3670,7 @@
         <v>85</v>
       </c>
       <c r="M46" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="N46" s="16">
         <v>51.2</v>
@@ -3684,7 +3684,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C47" s="20">
         <v>10942</v>
@@ -3712,7 +3712,7 @@
         <v>84</v>
       </c>
       <c r="M47" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N47" s="16">
         <v>35.72</v>
@@ -3726,7 +3726,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C48" s="18">
         <v>6020</v>
@@ -3747,7 +3747,7 @@
         <v>45317</v>
       </c>
       <c r="I48" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J48" s="24">
         <v>36284</v>
@@ -3757,7 +3757,7 @@
         <v>85</v>
       </c>
       <c r="M48" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N48" s="16">
         <v>44.48</v>
@@ -3771,7 +3771,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C49" s="18">
         <v>10038</v>
@@ -3792,7 +3792,7 @@
         <v>45317</v>
       </c>
       <c r="I49" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J49" s="24">
         <v>33386</v>
@@ -3802,7 +3802,7 @@
         <v>85</v>
       </c>
       <c r="M49" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="N49" s="16">
         <v>61.56</v>
@@ -3816,13 +3816,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C50" s="18">
         <v>6477</v>
       </c>
       <c r="D50" s="19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E50" s="1">
         <v>1</v>
@@ -3844,7 +3844,7 @@
         <v>83</v>
       </c>
       <c r="M50" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="N50" s="16">
         <v>45.46</v>
@@ -3867,12 +3867,12 @@
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="J53" s="16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="J54" s="16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Textgrid Speak pt. 46, Praat output
</commit_message>
<xml_diff>
--- a/REPSWITCH_List.xlsx
+++ b/REPSWITCH_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\experiment1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07782805-7D45-45CF-AE72-5928482AA2A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56EF4CD0-2A74-407B-941A-E3116DA2B3F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -598,27 +598,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -638,7 +621,13 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -650,6 +639,17 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1153,21 +1153,21 @@
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{6A81B45A-EDC9-4FF5-8258-8648C067C16F}" name="Participant"/>
     <tableColumn id="5" xr3:uid="{23D0A20D-D062-4D9A-A44D-D77B8E1CBB39}" name="Name"/>
-    <tableColumn id="10" xr3:uid="{706E71AC-2B72-418D-A17F-64B513C711DC}" name="ID" dataDxfId="17" totalsRowDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{7D21F159-CC51-40B5-A3A9-2FC35A1E3DC7}" name="Code" dataDxfId="16" totalsRowDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{706E71AC-2B72-418D-A17F-64B513C711DC}" name="ID" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{7D21F159-CC51-40B5-A3A9-2FC35A1E3DC7}" name="Code" dataDxfId="15" totalsRowDxfId="14"/>
     <tableColumn id="2" xr3:uid="{0F7B8E20-170E-4530-BD6F-052C78EE98C3}" name="Version "/>
     <tableColumn id="3" xr3:uid="{C9573F81-3819-423D-82CC-5ABB8EA301BD}" name="List"/>
-    <tableColumn id="6" xr3:uid="{27B86DF5-6EF1-41B1-A9EC-9F0F5F275ADB}" name="Language_test" dataDxfId="15" totalsRowDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{27B86DF5-6EF1-41B1-A9EC-9F0F5F275ADB}" name="Language_test" dataDxfId="13" totalsRowDxfId="12"/>
     <tableColumn id="9" xr3:uid="{89FF1955-3050-4A09-8388-44DB3C7BAF8D}" name="Date"/>
     <tableColumn id="13" xr3:uid="{0353A7A6-5360-4B04-A7A6-65360A0DB44E}" name="Notes"/>
-    <tableColumn id="14" xr3:uid="{4580F522-AB7C-463E-B145-EBE3420458C5}" name="FechaNacimiento" dataDxfId="14" totalsRowDxfId="5"/>
-    <tableColumn id="11" xr3:uid="{692F1DCA-E4E0-468B-99F8-ADCD8D7F70E7}" name="Age" dataDxfId="13" totalsRowDxfId="4"/>
-    <tableColumn id="15" xr3:uid="{E351B0AB-595F-4765-9989-9C66FD2C2557}" name="Sexo" dataDxfId="12" totalsRowDxfId="3"/>
-    <tableColumn id="16" xr3:uid="{C57334FC-C4FE-4E54-8FCF-DE2F9464D89B}" name="Supertecleador" dataDxfId="11" totalsRowDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{4C118AC6-F397-4959-8D77-72283767A378}" name="Type_speed" totalsRowFunction="custom" dataDxfId="10" totalsRowDxfId="1">
+    <tableColumn id="14" xr3:uid="{4580F522-AB7C-463E-B145-EBE3420458C5}" name="FechaNacimiento" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="11" xr3:uid="{692F1DCA-E4E0-468B-99F8-ADCD8D7F70E7}" name="Age" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="15" xr3:uid="{E351B0AB-595F-4765-9989-9C66FD2C2557}" name="Sexo" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="16" xr3:uid="{C57334FC-C4FE-4E54-8FCF-DE2F9464D89B}" name="Supertecleador" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{4C118AC6-F397-4959-8D77-72283767A378}" name="Type_speed" totalsRowFunction="custom" dataDxfId="3" totalsRowDxfId="2">
       <totalsRowFormula>AVERAGE(Table1[Type_speed])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{298D1824-20FA-4582-B3FC-14618C8BA8DE}" name="Type_accuracy" totalsRowFunction="custom" dataDxfId="9" totalsRowDxfId="0">
+    <tableColumn id="7" xr3:uid="{298D1824-20FA-4582-B3FC-14618C8BA8DE}" name="Type_accuracy" totalsRowFunction="custom" dataDxfId="1" totalsRowDxfId="0">
       <totalsRowFormula>AVERAGE(Table1[Type_accuracy])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -1632,8 +1632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{395959F8-4BC5-4C1E-B558-7BF10E8FA50A}">
   <dimension ref="A1:T54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>